<commit_message>
add view table lipa 24
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_24.xlsx
+++ b/hasil/2023_01_lipa_24.xlsx
@@ -59,7 +59,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 10 Agustus 2023</t>
+    <t>Ternate , 11 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -576,7 +576,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -801,7 +801,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" customHeight="1" ht="90">
+    <row r="9" spans="1:19" customHeight="1" ht="65">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -882,10 +882,10 @@
     </row>
     <row r="12" spans="1:19" customHeight="1" ht="20">
       <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -907,10 +907,10 @@
     </row>
     <row r="13" spans="1:19" customHeight="1" ht="20">
       <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1016,10 +1016,10 @@
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="20">
       <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>17</v>
       </c>
+      <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -1041,10 +1041,10 @@
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="20">
       <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>

</xml_diff>